<commit_message>
data preparation and visualisation
</commit_message>
<xml_diff>
--- a/CorrelationAnalysis/data/european_population.xlsx
+++ b/CorrelationAnalysis/data/european_population.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osi0pr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osi0pr\Documents\Github\Masterarbeit\CorrelationAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382B80D8-699F-4144-A1B3-D90E9F08D5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFD785-CC84-457E-9A03-31224835FAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Belgium</t>
   </si>
@@ -646,7 +646,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2004,8 +2004,8 @@
       <c r="L33" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M33" s="5" t="s">
-        <v>62</v>
+      <c r="M33" s="5">
+        <v>67736802</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adapted Patent and Stations data, updated grpahics etc
</commit_message>
<xml_diff>
--- a/CorrelationAnalysis/data/european_population.xlsx
+++ b/CorrelationAnalysis/data/european_population.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osi0pr\Documents\Github\Masterarbeit\CorrelationAnalysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.premstaller\Documents\Github\Masterarbeit\CorrelationAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AFD785-CC84-457E-9A03-31224835FAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A87D8E7-10E2-4460-A3BE-C237B894F73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="3" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Bulgaria</t>
   </si>
   <si>
-    <t>Czechia</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Serbia</t>
   </si>
   <si>
-    <t>Türkiye</t>
-  </si>
-  <si>
     <t>Andorra</t>
   </si>
   <si>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>:</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -646,57 +646,57 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M34" sqref="M34"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.90625" customWidth="1"/>
     <col min="2" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -737,7 +737,7 @@
         <v>11742796</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -778,9 +778,9 @@
         <v>6447710</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5">
         <v>10505445</v>
@@ -819,9 +819,9 @@
         <v>10827529</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4">
         <v>5580516</v>
@@ -860,9 +860,9 @@
         <v>5932654</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5">
         <v>80327900</v>
@@ -901,9 +901,9 @@
         <v>84358845</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
         <v>1325217</v>
@@ -942,9 +942,9 @@
         <v>1365884</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5">
         <v>4589287</v>
@@ -983,9 +983,9 @@
         <v>5271395</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4">
         <v>11086406</v>
@@ -1024,9 +1024,9 @@
         <v>10413982</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>46818219</v>
@@ -1065,9 +1065,9 @@
         <v>48085361</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4">
         <v>65276983</v>
@@ -1106,9 +1106,9 @@
         <v>68172977</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>4275984</v>
@@ -1147,9 +1147,9 @@
         <v>3850894</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5">
         <v>59394207</v>
@@ -1188,9 +1188,9 @@
         <v>58997201</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="4">
         <v>862011</v>
@@ -1229,9 +1229,9 @@
         <v>920701</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5">
         <v>2044813</v>
@@ -1270,9 +1270,9 @@
         <v>1883008</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4">
         <v>3003641</v>
@@ -1311,9 +1311,9 @@
         <v>2857279</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5">
         <v>524853</v>
@@ -1352,9 +1352,9 @@
         <v>660809</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>9931925</v>
@@ -1393,9 +1393,9 @@
         <v>9599744</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="5">
         <v>417546</v>
@@ -1434,9 +1434,9 @@
         <v>542051</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4">
         <v>16730348</v>
@@ -1475,9 +1475,9 @@
         <v>17811291</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="5">
         <v>8408121</v>
@@ -1516,9 +1516,9 @@
         <v>9104772</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4">
         <v>38063792</v>
@@ -1557,9 +1557,9 @@
         <v>36753736</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5">
         <v>10542398</v>
@@ -1598,9 +1598,9 @@
         <v>10467366</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4">
         <v>20095996</v>
@@ -1639,9 +1639,9 @@
         <v>19054548</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="5">
         <v>2055496</v>
@@ -1680,9 +1680,9 @@
         <v>2116972</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="4">
         <v>5404322</v>
@@ -1721,9 +1721,9 @@
         <v>5428792</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5">
         <v>5401267</v>
@@ -1762,9 +1762,9 @@
         <v>5563970</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="4">
         <v>9482855</v>
@@ -1803,9 +1803,9 @@
         <v>10521556</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="5">
         <v>319575</v>
@@ -1844,9 +1844,9 @@
         <v>387758</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4">
         <v>36475</v>
@@ -1885,9 +1885,9 @@
         <v>39677</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="5">
         <v>4985870</v>
@@ -1926,9 +1926,9 @@
         <v>5488984</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4">
         <v>7954662</v>
@@ -1967,9 +1967,9 @@
         <v>8815385</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5">
         <v>63495088</v>
@@ -1999,18 +1999,18 @@
         <v>67025542</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L33" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M33" s="5">
         <v>67736802</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="4">
         <v>620308</v>
@@ -2049,9 +2049,9 @@
         <v>616695</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5">
         <v>2059794</v>
@@ -2090,9 +2090,9 @@
         <v>1829954</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="4">
         <v>2903008</v>
@@ -2131,9 +2131,9 @@
         <v>2761785</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5">
         <v>7216649</v>
@@ -2172,9 +2172,9 @@
         <v>6641197</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B38" s="4">
         <v>74724269</v>
@@ -2213,9 +2213,9 @@
         <v>85279553</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B39" s="5">
         <v>78115</v>
@@ -2224,16 +2224,16 @@
         <v>76246</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F39" s="5">
         <v>71732</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H39" s="5">
         <v>74794</v>
@@ -2245,7 +2245,7 @@
         <v>77543</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L39" s="5">
         <v>79535</v>
@@ -2254,9 +2254,9 @@
         <v>81588</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="4">
         <v>9465150</v>
@@ -2286,18 +2286,18 @@
         <v>9408350</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41" s="5">
         <v>3839265</v>
@@ -2324,21 +2324,21 @@
         <v>3492018</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42" s="4">
         <v>1780021</v>
@@ -2371,15 +2371,15 @@
         <v>1798188</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" s="5">
         <v>3559541</v>
@@ -2418,18 +2418,18 @@
         <v>2512758</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E44" s="4">
         <v>37700</v>
@@ -2438,7 +2438,7 @@
         <v>38200</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H44" s="4">
         <v>38300</v>
@@ -2447,62 +2447,62 @@
         <v>38300</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" s="5">
         <v>143056383</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D45" s="5">
         <v>143666931</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46" s="4">
         <v>33376</v>
@@ -2541,9 +2541,9 @@
         <v>33812</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47" s="5">
         <v>45453282</v>
@@ -2573,18 +2573,18 @@
         <v>41732779</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L47" s="5">
         <v>40997698</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48" s="4">
         <v>3274285</v>
@@ -2617,15 +2617,15 @@
         <v>2963251</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M48" s="4">
         <v>2977130</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" s="5">
         <v>9235085</v>
@@ -2664,15 +2664,15 @@
         <v>10127145</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50" s="4">
         <v>4497617</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D50" s="4">
         <v>4490498</v>

</xml_diff>